<commit_message>
Ajuste de escaleta tema 7
Ajuste de escaleta tema 07 sexto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion07/Escaleta_MA_06_07_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion07/Escaleta_MA_06_07_CO.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1575" windowWidth="20730" windowHeight="11700"/>
+    <workbookView xWindow="1920" yWindow="1580" windowWidth="23420" windowHeight="13960"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$37</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="140001" iterateCount="2" iterateDelta="10" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -620,9 +620,6 @@
     <t>El recurso no tiene modificaciones.</t>
   </si>
   <si>
-    <t>Explicar la comparación de decimales utilizando la recta numérica, proponer la comparación de fracciones con decimales y decimales con decimales. Plantear los ejercicios de práctica.</t>
-  </si>
-  <si>
     <t>Recurso F6B-01</t>
   </si>
   <si>
@@ -744,12 +741,6 @@
   </si>
   <si>
     <t>Actividad para practicar el truncamiento de números decimales</t>
-  </si>
-  <si>
-    <t>Comparación de números decimales</t>
-  </si>
-  <si>
-    <t>Interactivo que explica la comparación de fracciones utilizando la recta numérica</t>
   </si>
   <si>
     <t>En la imagen presentar la recta numérica ubicando un punto y en las respuestas el decimal localizado.</t>
@@ -970,14 +961,42 @@
       <t>os porcentajes en la solución de problemas</t>
     </r>
   </si>
+  <si>
+    <t>Representación de números decimales en la recta</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Interactivo que explica </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>el uso de la recta numérica en los decimales</t>
+    </r>
+  </si>
+  <si>
+    <t>Explicar cómo se ubican decimales en la recta, tener en cuenta una cifra decimal, dos cifras decimales y tres cifras decimales. Generalizar la forma de ubicar cualquier decimal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1269,180 +1288,189 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1756,23 +1784,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" style="9"/>
     <col min="2" max="2" width="22" style="9" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" style="24" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="25" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="61.140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="25" customWidth="1"/>
+    <col min="7" max="7" width="61.1640625" style="10" customWidth="1"/>
     <col min="8" max="9" width="14" style="10"/>
-    <col min="10" max="10" width="61.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="61.83203125" style="9" customWidth="1"/>
     <col min="11" max="14" width="14" style="9"/>
-    <col min="15" max="15" width="39.42578125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="39.5" style="9" customWidth="1"/>
     <col min="16" max="16" width="16" style="10" customWidth="1"/>
     <col min="17" max="19" width="14" style="10"/>
     <col min="20" max="20" width="37" style="34" customWidth="1"/>
@@ -1780,82 +1808,82 @@
     <col min="22" max="16384" width="14" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:21" ht="15" customHeight="1">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>270</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="53" t="s">
         <v>271</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="I1" s="55" t="s">
         <v>272</v>
       </c>
-      <c r="F1" s="48" t="s">
-        <v>273</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="50" t="s">
-        <v>274</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>275</v>
-      </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="L1" s="38" t="s">
+      <c r="K1" s="42" t="s">
+        <v>267</v>
+      </c>
+      <c r="L1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="42"/>
+      <c r="N1" s="45"/>
       <c r="O1" s="35" t="s">
         <v>111</v>
       </c>
       <c r="P1" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="Q1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="55" t="s">
+      <c r="T1" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="54" t="s">
+      <c r="U1" s="36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="38"/>
+    <row r="2" spans="1:21" ht="15" customHeight="1">
+      <c r="A2" s="40"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="41"/>
       <c r="M2" s="1" t="s">
         <v>39</v>
       </c>
@@ -1864,13 +1892,13 @@
       </c>
       <c r="O2" s="35"/>
       <c r="P2" s="35"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="54"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q2" s="36"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="36"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1888,7 +1916,7 @@
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="30" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H3" s="28">
         <v>1</v>
@@ -1897,7 +1925,7 @@
         <v>134</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>114</v>
@@ -1931,7 +1959,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1951,7 +1979,7 @@
         <v>140</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H4" s="29">
         <v>2</v>
@@ -1973,7 +2001,7 @@
         <v>47</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="P4" s="22" t="s">
         <v>134</v>
@@ -1994,7 +2022,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -2014,7 +2042,7 @@
         <v>119</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H5" s="28">
         <v>3</v>
@@ -2036,7 +2064,7 @@
         <v>21</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="P5" s="22" t="s">
         <v>134</v>
@@ -2057,7 +2085,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -2071,7 +2099,7 @@
         <v>116</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>119</v>
@@ -2118,7 +2146,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2145,7 +2173,7 @@
         <v>134</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>134</v>
@@ -2177,7 +2205,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2202,7 +2230,7 @@
         <v>114</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>134</v>
@@ -2234,7 +2262,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2252,7 +2280,7 @@
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="31" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H9" s="28">
         <v>7</v>
@@ -2293,7 +2321,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -2320,7 +2348,7 @@
         <v>114</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>114</v>
@@ -2333,7 +2361,7 @@
         <v>42</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P10" s="22" t="s">
         <v>134</v>
@@ -2354,7 +2382,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -2372,7 +2400,7 @@
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="31" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H11" s="28">
         <v>9</v>
@@ -2392,7 +2420,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P11" s="22" t="s">
         <v>134</v>
@@ -2413,7 +2441,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -2449,7 +2477,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P12" s="22" t="s">
         <v>134</v>
@@ -2470,7 +2498,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -2488,7 +2516,7 @@
       </c>
       <c r="F13" s="27"/>
       <c r="G13" s="31" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H13" s="28">
         <v>11</v>
@@ -2497,7 +2525,7 @@
         <v>114</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>114</v>
@@ -2531,7 +2559,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -2551,7 +2579,7 @@
         <v>127</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H14" s="29">
         <v>12</v>
@@ -2560,7 +2588,7 @@
         <v>114</v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K14" s="5" t="s">
         <v>113</v>
@@ -2571,7 +2599,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P14" s="22" t="s">
         <v>114</v>
@@ -2592,7 +2620,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -2653,7 +2681,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -2712,7 +2740,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -2771,7 +2799,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2782,12 +2810,12 @@
         <v>151</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="27"/>
       <c r="G18" s="32" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H18" s="29">
         <v>16</v>
@@ -2796,7 +2824,7 @@
         <v>134</v>
       </c>
       <c r="J18" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>114</v>
@@ -2809,7 +2837,7 @@
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P18" s="22" t="s">
         <v>134</v>
@@ -2824,13 +2852,13 @@
         <v>137</v>
       </c>
       <c r="T18" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U18" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -2841,7 +2869,7 @@
         <v>151</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>129</v>
@@ -2857,7 +2885,7 @@
         <v>114</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>114</v>
@@ -2891,7 +2919,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2902,7 +2930,7 @@
         <v>151</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>130</v>
@@ -2952,7 +2980,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2963,7 +2991,7 @@
         <v>151</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="27"/>
@@ -3009,7 +3037,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -3020,12 +3048,12 @@
         <v>151</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="27"/>
       <c r="G22" s="32" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H22" s="29">
         <v>20</v>
@@ -3068,7 +3096,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -3079,14 +3107,14 @@
         <v>151</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>123</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="31" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H23" s="28">
         <v>21</v>
@@ -3129,7 +3157,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -3140,12 +3168,12 @@
         <v>151</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="31" t="s">
-        <v>240</v>
+      <c r="G24" s="57" t="s">
+        <v>279</v>
       </c>
       <c r="H24" s="29">
         <v>22</v>
@@ -3153,8 +3181,8 @@
       <c r="I24" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="J24" s="21" t="s">
-        <v>241</v>
+      <c r="J24" s="58" t="s">
+        <v>280</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>114</v>
@@ -3166,8 +3194,8 @@
         <v>13</v>
       </c>
       <c r="N24" s="6"/>
-      <c r="O24" s="14" t="s">
-        <v>198</v>
+      <c r="O24" s="59" t="s">
+        <v>281</v>
       </c>
       <c r="P24" s="22" t="s">
         <v>114</v>
@@ -3182,13 +3210,13 @@
         <v>137</v>
       </c>
       <c r="T24" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U24" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -3199,12 +3227,12 @@
         <v>151</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="27"/>
       <c r="G25" s="31" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H25" s="28">
         <v>23</v>
@@ -3213,7 +3241,7 @@
         <v>114</v>
       </c>
       <c r="J25" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>114</v>
@@ -3226,7 +3254,7 @@
         <v>52</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="P25" s="22" t="s">
         <v>134</v>
@@ -3241,13 +3269,13 @@
         <v>143</v>
       </c>
       <c r="T25" s="33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U25" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -3258,14 +3286,14 @@
         <v>151</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>123</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="31" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H26" s="29">
         <v>24</v>
@@ -3274,7 +3302,7 @@
         <v>114</v>
       </c>
       <c r="J26" s="21" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>114</v>
@@ -3287,7 +3315,7 @@
         <v>31</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="P26" s="22" t="s">
         <v>134</v>
@@ -3302,13 +3330,13 @@
         <v>143</v>
       </c>
       <c r="T26" s="33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U26" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -3324,7 +3352,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="27"/>
       <c r="G27" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H27" s="28">
         <v>25</v>
@@ -3333,7 +3361,7 @@
         <v>114</v>
       </c>
       <c r="J27" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>134</v>
@@ -3359,13 +3387,13 @@
         <v>151</v>
       </c>
       <c r="T27" s="33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U27" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
@@ -3381,7 +3409,7 @@
       <c r="E28" s="20"/>
       <c r="F28" s="27"/>
       <c r="G28" s="31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H28" s="29">
         <v>26</v>
@@ -3390,7 +3418,7 @@
         <v>114</v>
       </c>
       <c r="J28" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>134</v>
@@ -3416,13 +3444,13 @@
         <v>151</v>
       </c>
       <c r="T28" s="33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="U28" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
@@ -3440,7 +3468,7 @@
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="31" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H29" s="28">
         <v>27</v>
@@ -3449,7 +3477,7 @@
         <v>114</v>
       </c>
       <c r="J29" s="21" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>114</v>
@@ -3462,7 +3490,7 @@
         <v>31</v>
       </c>
       <c r="O29" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P29" s="22" t="s">
         <v>134</v>
@@ -3477,13 +3505,13 @@
         <v>143</v>
       </c>
       <c r="T29" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U29" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
@@ -3499,7 +3527,7 @@
       <c r="E30" s="20"/>
       <c r="F30" s="27"/>
       <c r="G30" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H30" s="29">
         <v>28</v>
@@ -3508,7 +3536,7 @@
         <v>134</v>
       </c>
       <c r="J30" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>114</v>
@@ -3521,7 +3549,7 @@
       </c>
       <c r="N30" s="6"/>
       <c r="O30" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P30" s="22" t="s">
         <v>134</v>
@@ -3536,13 +3564,13 @@
         <v>137</v>
       </c>
       <c r="T30" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U30" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
@@ -3558,7 +3586,7 @@
       <c r="E31" s="20"/>
       <c r="F31" s="27"/>
       <c r="G31" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H31" s="28">
         <v>29</v>
@@ -3567,7 +3595,7 @@
         <v>114</v>
       </c>
       <c r="J31" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>114</v>
@@ -3580,7 +3608,7 @@
         <v>51</v>
       </c>
       <c r="O31" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P31" s="22" t="s">
         <v>134</v>
@@ -3595,13 +3623,13 @@
         <v>143</v>
       </c>
       <c r="T31" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U31" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>7</v>
       </c>
@@ -3619,7 +3647,7 @@
       </c>
       <c r="F32" s="27"/>
       <c r="G32" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H32" s="29">
         <v>30</v>
@@ -3628,7 +3656,7 @@
         <v>114</v>
       </c>
       <c r="J32" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>114</v>
@@ -3641,7 +3669,7 @@
         <v>31</v>
       </c>
       <c r="O32" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P32" s="22" t="s">
         <v>134</v>
@@ -3656,13 +3684,13 @@
         <v>143</v>
       </c>
       <c r="T32" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="U32" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
@@ -3678,7 +3706,7 @@
       <c r="E33" s="20"/>
       <c r="F33" s="27"/>
       <c r="G33" s="32" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H33" s="28">
         <v>31</v>
@@ -3687,7 +3715,7 @@
         <v>114</v>
       </c>
       <c r="J33" s="21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>114</v>
@@ -3700,7 +3728,7 @@
         <v>33</v>
       </c>
       <c r="O33" s="14" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="P33" s="22" t="s">
         <v>134</v>
@@ -3715,13 +3743,13 @@
         <v>143</v>
       </c>
       <c r="T33" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U33" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
@@ -3737,7 +3765,7 @@
       <c r="E34" s="20"/>
       <c r="F34" s="27"/>
       <c r="G34" s="32" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H34" s="29">
         <v>32</v>
@@ -3746,7 +3774,7 @@
         <v>114</v>
       </c>
       <c r="J34" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>114</v>
@@ -3759,7 +3787,7 @@
         <v>33</v>
       </c>
       <c r="O34" s="14" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="P34" s="22" t="s">
         <v>134</v>
@@ -3774,13 +3802,13 @@
         <v>143</v>
       </c>
       <c r="T34" s="33" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="U34" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
@@ -3794,7 +3822,7 @@
       <c r="E35" s="20"/>
       <c r="F35" s="27"/>
       <c r="G35" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H35" s="28">
         <v>33</v>
@@ -3803,7 +3831,7 @@
         <v>114</v>
       </c>
       <c r="J35" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>114</v>
@@ -3814,7 +3842,7 @@
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="O35" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P35" s="22" t="s">
         <v>134</v>
@@ -3825,7 +3853,7 @@
       <c r="T35" s="33"/>
       <c r="U35" s="18"/>
     </row>
-    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -3839,7 +3867,7 @@
       <c r="E36" s="20"/>
       <c r="F36" s="27"/>
       <c r="G36" s="31" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H36" s="29">
         <v>34</v>
@@ -3848,7 +3876,7 @@
         <v>114</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>114</v>
@@ -3861,7 +3889,7 @@
         <v>52</v>
       </c>
       <c r="O36" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P36" s="22" t="s">
         <v>134</v>
@@ -3876,13 +3904,13 @@
         <v>143</v>
       </c>
       <c r="T36" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U36" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>7</v>
       </c>
@@ -3896,7 +3924,7 @@
       <c r="E37" s="20"/>
       <c r="F37" s="27"/>
       <c r="G37" s="31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H37" s="28">
         <v>35</v>
@@ -3916,7 +3944,7 @@
         <v>32</v>
       </c>
       <c r="O37" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P37" s="22" t="s">
         <v>114</v>
@@ -3931,16 +3959,16 @@
         <v>143</v>
       </c>
       <c r="T37" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U37" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="15" customHeight="1">
       <c r="D40" s="10"/>
     </row>
-    <row r="78" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15" customHeight="1">
       <c r="A78" s="9" t="s">
         <v>34</v>
       </c>
@@ -3957,62 +3985,62 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15" customHeight="1">
       <c r="A80" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15" customHeight="1">
       <c r="A81" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15" customHeight="1">
       <c r="A82" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15" customHeight="1">
       <c r="A83" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="15" customHeight="1">
       <c r="A84" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="15" customHeight="1">
       <c r="A85" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="15" customHeight="1">
       <c r="A86" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="15" customHeight="1">
       <c r="A87" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="15" customHeight="1">
       <c r="A88" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15" customHeight="1">
       <c r="A89" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15" customHeight="1">
       <c r="A90" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="15" customHeight="1">
       <c r="A91" s="9" t="s">
         <v>52</v>
       </c>
@@ -4020,7 +4048,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="15" customHeight="1">
       <c r="A92" s="9" t="s">
         <v>53</v>
       </c>
@@ -4028,7 +4056,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="15" customHeight="1">
       <c r="A93" s="9" t="s">
         <v>54</v>
       </c>
@@ -4036,7 +4064,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="15" customHeight="1">
       <c r="A94" s="9" t="s">
         <v>55</v>
       </c>
@@ -4044,7 +4072,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="15" customHeight="1">
       <c r="A95" s="9" t="s">
         <v>14</v>
       </c>
@@ -4052,7 +4080,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="15" customHeight="1">
       <c r="A96" s="9" t="s">
         <v>15</v>
       </c>
@@ -4060,7 +4088,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15" customHeight="1">
       <c r="A97" s="9" t="s">
         <v>16</v>
       </c>
@@ -4068,7 +4096,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15" customHeight="1">
       <c r="A98" s="9" t="s">
         <v>17</v>
       </c>
@@ -4076,7 +4104,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="15" customHeight="1">
       <c r="A99" s="9" t="s">
         <v>18</v>
       </c>
@@ -4084,7 +4112,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15" customHeight="1">
       <c r="A100" s="9" t="s">
         <v>19</v>
       </c>
@@ -4092,7 +4120,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15" customHeight="1">
       <c r="A101" s="9" t="s">
         <v>20</v>
       </c>
@@ -4100,7 +4128,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="15" customHeight="1">
       <c r="A102" s="9" t="s">
         <v>21</v>
       </c>
@@ -4108,7 +4136,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="15" customHeight="1">
       <c r="A103" s="9" t="s">
         <v>22</v>
       </c>
@@ -4116,7 +4144,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15" customHeight="1">
       <c r="A104" s="9" t="s">
         <v>23</v>
       </c>
@@ -4124,7 +4152,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15" customHeight="1">
       <c r="A105" s="9" t="s">
         <v>24</v>
       </c>
@@ -4132,7 +4160,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15" customHeight="1">
       <c r="A106" s="9" t="s">
         <v>25</v>
       </c>
@@ -4140,7 +4168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15" customHeight="1">
       <c r="A107" s="9" t="s">
         <v>26</v>
       </c>
@@ -4148,7 +4176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="15" customHeight="1">
       <c r="A108" s="9" t="s">
         <v>27</v>
       </c>
@@ -4156,7 +4184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="15" customHeight="1">
       <c r="A109" s="9" t="s">
         <v>28</v>
       </c>
@@ -4164,7 +4192,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15" customHeight="1">
       <c r="A110" s="9" t="s">
         <v>29</v>
       </c>
@@ -4172,7 +4200,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="15" customHeight="1">
       <c r="A111" s="9" t="s">
         <v>30</v>
       </c>
@@ -4180,7 +4208,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15" customHeight="1">
       <c r="A112" s="9" t="s">
         <v>31</v>
       </c>
@@ -4188,7 +4216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="15" customHeight="1">
       <c r="A113" s="9" t="s">
         <v>32</v>
       </c>
@@ -4196,7 +4224,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="15" customHeight="1">
       <c r="A114" s="9" t="s">
         <v>33</v>
       </c>
@@ -4204,7 +4232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="15" customHeight="1">
       <c r="A115" s="9" t="s">
         <v>56</v>
       </c>
@@ -4212,7 +4240,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="15" customHeight="1">
       <c r="A116" s="9" t="s">
         <v>57</v>
       </c>
@@ -4220,7 +4248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="15" customHeight="1">
       <c r="A117" s="9" t="s">
         <v>58</v>
       </c>
@@ -4228,7 +4256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="15" customHeight="1">
       <c r="A118" s="9" t="s">
         <v>59</v>
       </c>
@@ -4236,7 +4264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="15" customHeight="1">
       <c r="A119" s="9" t="s">
         <v>60</v>
       </c>
@@ -4244,7 +4272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="15" customHeight="1">
       <c r="A120" s="9" t="s">
         <v>61</v>
       </c>
@@ -4252,7 +4280,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="15" customHeight="1">
       <c r="A121" s="9" t="s">
         <v>62</v>
       </c>
@@ -4260,7 +4288,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="15" customHeight="1">
       <c r="A122" s="9" t="s">
         <v>63</v>
       </c>
@@ -4268,7 +4296,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="15" customHeight="1">
       <c r="A123" s="9" t="s">
         <v>64</v>
       </c>
@@ -4276,7 +4304,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="15" customHeight="1">
       <c r="A124" s="9" t="s">
         <v>65</v>
       </c>
@@ -4284,7 +4312,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="15" customHeight="1">
       <c r="A125" s="9" t="s">
         <v>66</v>
       </c>
@@ -4292,7 +4320,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="15" customHeight="1">
       <c r="A126" s="9" t="s">
         <v>67</v>
       </c>
@@ -4300,7 +4328,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="15" customHeight="1">
       <c r="A127" s="9" t="s">
         <v>68</v>
       </c>
@@ -4308,7 +4336,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="15" customHeight="1">
       <c r="A128" s="9" t="s">
         <v>69</v>
       </c>
@@ -4316,7 +4344,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="15" customHeight="1">
       <c r="A129" s="9" t="s">
         <v>70</v>
       </c>
@@ -4324,7 +4352,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="15" customHeight="1">
       <c r="A130" s="9" t="s">
         <v>71</v>
       </c>
@@ -4332,7 +4360,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="15" customHeight="1">
       <c r="A131" s="9" t="s">
         <v>72</v>
       </c>
@@ -4340,7 +4368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="15" customHeight="1">
       <c r="A132" s="9" t="s">
         <v>73</v>
       </c>
@@ -4348,7 +4376,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="15" customHeight="1">
       <c r="A133" s="9" t="s">
         <v>74</v>
       </c>
@@ -4356,7 +4384,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="15" customHeight="1">
       <c r="A134" s="9" t="s">
         <v>75</v>
       </c>
@@ -4364,7 +4392,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="15" customHeight="1">
       <c r="A135" s="9" t="s">
         <v>76</v>
       </c>
@@ -4372,7 +4400,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="15" customHeight="1">
       <c r="A136" s="9" t="s">
         <v>77</v>
       </c>
@@ -4380,7 +4408,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="15" customHeight="1">
       <c r="A137" s="9" t="s">
         <v>78</v>
       </c>
@@ -4388,7 +4416,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="15" customHeight="1">
       <c r="A138" s="9" t="s">
         <v>79</v>
       </c>
@@ -4396,7 +4424,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="15" customHeight="1">
       <c r="A139" s="9" t="s">
         <v>80</v>
       </c>
@@ -4404,7 +4432,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="15" customHeight="1">
       <c r="A140" s="9" t="s">
         <v>81</v>
       </c>
@@ -4412,7 +4440,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="15" customHeight="1">
       <c r="A141" s="9" t="s">
         <v>82</v>
       </c>
@@ -4420,7 +4448,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="15" customHeight="1">
       <c r="A142" s="9" t="s">
         <v>83</v>
       </c>
@@ -4428,7 +4456,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="15" customHeight="1">
       <c r="A143" s="9" t="s">
         <v>84</v>
       </c>
@@ -4436,7 +4464,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="15" customHeight="1">
       <c r="A144" s="9" t="s">
         <v>85</v>
       </c>
@@ -4444,7 +4472,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="15" customHeight="1">
       <c r="A145" s="9" t="s">
         <v>86</v>
       </c>
@@ -4452,7 +4480,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="15" customHeight="1">
       <c r="A146" s="9" t="s">
         <v>87</v>
       </c>
@@ -4460,7 +4488,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="15" customHeight="1">
       <c r="A147" s="9" t="s">
         <v>88</v>
       </c>
@@ -4468,7 +4496,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="15" customHeight="1">
       <c r="A148" s="9" t="s">
         <v>89</v>
       </c>
@@ -4476,7 +4504,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="15" customHeight="1">
       <c r="A149" s="9" t="s">
         <v>90</v>
       </c>
@@ -4484,7 +4512,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="15" customHeight="1">
       <c r="A150" s="9" t="s">
         <v>91</v>
       </c>
@@ -4492,7 +4520,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="15" customHeight="1">
       <c r="A151" s="9" t="s">
         <v>92</v>
       </c>
@@ -4500,7 +4528,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="15" customHeight="1">
       <c r="A152" s="9" t="s">
         <v>93</v>
       </c>
@@ -4508,7 +4536,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="15" customHeight="1">
       <c r="A153" s="9" t="s">
         <v>94</v>
       </c>
@@ -4516,7 +4544,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="15" customHeight="1">
       <c r="A154" s="9" t="s">
         <v>95</v>
       </c>
@@ -4524,7 +4552,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="15" customHeight="1">
       <c r="A155" s="9" t="s">
         <v>96</v>
       </c>
@@ -4532,7 +4560,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="15" customHeight="1">
       <c r="A156" s="9" t="s">
         <v>97</v>
       </c>
@@ -4540,7 +4568,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="15" customHeight="1">
       <c r="A157" s="9" t="s">
         <v>98</v>
       </c>
@@ -4548,7 +4576,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="15" customHeight="1">
       <c r="A158" s="9" t="s">
         <v>99</v>
       </c>
@@ -4556,7 +4584,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="15" customHeight="1">
       <c r="A159" s="9" t="s">
         <v>100</v>
       </c>
@@ -4564,7 +4592,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="15" customHeight="1">
       <c r="A160" s="9" t="s">
         <v>101</v>
       </c>
@@ -4572,7 +4600,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="15" customHeight="1">
       <c r="A161" s="9" t="s">
         <v>102</v>
       </c>
@@ -4580,7 +4608,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="15" customHeight="1">
       <c r="A162" s="9" t="s">
         <v>103</v>
       </c>
@@ -4588,7 +4616,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="15" customHeight="1">
       <c r="A163" s="9" t="s">
         <v>104</v>
       </c>
@@ -4596,7 +4624,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="15" customHeight="1">
       <c r="A164" s="9" t="s">
         <v>105</v>
       </c>
@@ -4604,7 +4632,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="15" customHeight="1">
       <c r="A165" s="9" t="s">
         <v>106</v>
       </c>
@@ -4612,7 +4640,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="15" customHeight="1">
       <c r="A166" s="9" t="s">
         <v>107</v>
       </c>
@@ -4620,7 +4648,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="15" customHeight="1">
       <c r="A167" s="9" t="s">
         <v>108</v>
       </c>
@@ -4628,7 +4656,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="15" customHeight="1">
       <c r="A168" s="9" t="s">
         <v>109</v>
       </c>
@@ -4636,7 +4664,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="15" customHeight="1">
       <c r="A169" s="9" t="s">
         <v>110</v>
       </c>
@@ -4644,69 +4672,63 @@
         <v>99</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="15" customHeight="1">
       <c r="G170" s="10" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="15" customHeight="1">
       <c r="G171" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="15" customHeight="1">
       <c r="G172" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="15" customHeight="1">
       <c r="G173" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="15" customHeight="1">
       <c r="G174" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="15" customHeight="1">
       <c r="G175" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="15" customHeight="1">
       <c r="G176" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="177" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="7:7" ht="15" customHeight="1">
       <c r="G177" s="10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="178" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="7:7" ht="15" customHeight="1">
       <c r="G178" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="179" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="7:7" ht="15" customHeight="1">
       <c r="G179" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="180" spans="7:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="7:7" ht="15" customHeight="1">
       <c r="G180" s="10" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -4721,6 +4743,12 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A37">
@@ -4743,7 +4771,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4758,7 +4785,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Ajuste escaleta tema 07
Ajuste escaleta tema 07
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion07/Escaleta_MA_06_07_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion07/Escaleta_MA_06_07_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1580" windowWidth="23420" windowHeight="13960"/>
+    <workbookView xWindow="1100" yWindow="0" windowWidth="25040" windowHeight="14020"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="283">
   <si>
     <t>Asignatura</t>
   </si>
@@ -759,9 +759,6 @@
   </si>
   <si>
     <t>Plantear en la imagen la fracción decimal y en las opciones de selección la expresión decimal.</t>
-  </si>
-  <si>
-    <t>Los decimales  en fracciones</t>
   </si>
   <si>
     <t>Interactivo que muestra una secuencia de imágenes que explica los ordenes de unidades de un número decimal</t>
@@ -982,14 +979,27 @@
   <si>
     <t>Explicar cómo se ubican decimales en la recta, tener en cuenta una cifra decimal, dos cifras decimales y tres cifras decimales. Generalizar la forma de ubicar cualquier decimal</t>
   </si>
+  <si>
+    <t>Los decimales y otras fracciones</t>
+  </si>
+  <si>
+    <t>Conversión entre fracciones y decimales</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1288,189 +1298,189 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1784,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F3" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1794,8 +1804,8 @@
     <col min="2" max="2" width="22" style="9" customWidth="1"/>
     <col min="3" max="3" width="44.1640625" style="9" customWidth="1"/>
     <col min="4" max="4" width="56.6640625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="25" customWidth="1"/>
+    <col min="5" max="5" width="39.5" style="25" customWidth="1"/>
+    <col min="6" max="6" width="41.5" style="25" customWidth="1"/>
     <col min="7" max="7" width="61.1640625" style="10" customWidth="1"/>
     <col min="8" max="9" width="14" style="10"/>
     <col min="10" max="10" width="61.83203125" style="9" customWidth="1"/>
@@ -1819,28 +1829,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="E1" s="49" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="F1" s="51" t="s">
         <v>269</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>270</v>
       </c>
       <c r="G1" s="41" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="53" t="s">
+        <v>270</v>
+      </c>
+      <c r="I1" s="55" t="s">
         <v>271</v>
-      </c>
-      <c r="I1" s="55" t="s">
-        <v>272</v>
       </c>
       <c r="J1" s="43" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L1" s="41" t="s">
         <v>5</v>
@@ -1849,25 +1859,25 @@
         <v>6</v>
       </c>
       <c r="N1" s="45"/>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="R1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="T1" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="57" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1890,13 +1900,13 @@
       <c r="N2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="36"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="57"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="57"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
@@ -1916,7 +1926,7 @@
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H3" s="28">
         <v>1</v>
@@ -1979,7 +1989,7 @@
         <v>140</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H4" s="29">
         <v>2</v>
@@ -2042,7 +2052,7 @@
         <v>119</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H5" s="28">
         <v>3</v>
@@ -2064,7 +2074,7 @@
         <v>21</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P5" s="22" t="s">
         <v>134</v>
@@ -2099,10 +2109,10 @@
         <v>116</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="G6" s="31" t="s">
         <v>195</v>
@@ -2173,7 +2183,7 @@
         <v>134</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>134</v>
@@ -2230,7 +2240,7 @@
         <v>114</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>134</v>
@@ -2280,7 +2290,7 @@
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H9" s="28">
         <v>7</v>
@@ -2348,7 +2358,7 @@
         <v>114</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>114</v>
@@ -2400,7 +2410,7 @@
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H11" s="28">
         <v>9</v>
@@ -2516,7 +2526,7 @@
       </c>
       <c r="F13" s="27"/>
       <c r="G13" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H13" s="28">
         <v>11</v>
@@ -2579,7 +2589,7 @@
         <v>127</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H14" s="29">
         <v>12</v>
@@ -2810,12 +2820,12 @@
         <v>151</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="27"/>
       <c r="G18" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H18" s="29">
         <v>16</v>
@@ -2869,7 +2879,7 @@
         <v>151</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>129</v>
@@ -2930,7 +2940,7 @@
         <v>151</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>130</v>
@@ -2991,7 +3001,7 @@
         <v>151</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="27"/>
@@ -3048,12 +3058,12 @@
         <v>151</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="27"/>
       <c r="G22" s="32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H22" s="29">
         <v>20</v>
@@ -3107,14 +3117,14 @@
         <v>151</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>123</v>
       </c>
       <c r="F23" s="27"/>
       <c r="G23" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H23" s="28">
         <v>21</v>
@@ -3168,12 +3178,12 @@
         <v>151</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="57" t="s">
-        <v>279</v>
+      <c r="G24" s="35" t="s">
+        <v>278</v>
       </c>
       <c r="H24" s="29">
         <v>22</v>
@@ -3181,8 +3191,8 @@
       <c r="I24" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="J24" s="58" t="s">
-        <v>280</v>
+      <c r="J24" s="36" t="s">
+        <v>279</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>114</v>
@@ -3194,8 +3204,8 @@
         <v>13</v>
       </c>
       <c r="N24" s="6"/>
-      <c r="O24" s="59" t="s">
-        <v>281</v>
+      <c r="O24" s="37" t="s">
+        <v>280</v>
       </c>
       <c r="P24" s="22" t="s">
         <v>114</v>
@@ -3227,12 +3237,12 @@
         <v>151</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="27"/>
       <c r="G25" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H25" s="28">
         <v>23</v>
@@ -3286,14 +3296,14 @@
         <v>151</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>123</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H26" s="29">
         <v>24</v>
@@ -3468,7 +3478,7 @@
       </c>
       <c r="F29" s="27"/>
       <c r="G29" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H29" s="28">
         <v>27</v>
@@ -3706,7 +3716,7 @@
       <c r="E33" s="20"/>
       <c r="F33" s="27"/>
       <c r="G33" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H33" s="28">
         <v>31</v>
@@ -3715,7 +3725,7 @@
         <v>114</v>
       </c>
       <c r="J33" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>114</v>
@@ -3728,7 +3738,7 @@
         <v>33</v>
       </c>
       <c r="O33" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P33" s="22" t="s">
         <v>134</v>
@@ -3765,7 +3775,7 @@
       <c r="E34" s="20"/>
       <c r="F34" s="27"/>
       <c r="G34" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H34" s="29">
         <v>32</v>
@@ -3787,7 +3797,7 @@
         <v>33</v>
       </c>
       <c r="O34" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P34" s="22" t="s">
         <v>134</v>
@@ -3802,7 +3812,7 @@
         <v>143</v>
       </c>
       <c r="T34" s="33" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U34" s="18" t="s">
         <v>145</v>
@@ -3831,7 +3841,7 @@
         <v>114</v>
       </c>
       <c r="J35" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>114</v>
@@ -3867,7 +3877,7 @@
       <c r="E36" s="20"/>
       <c r="F36" s="27"/>
       <c r="G36" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H36" s="29">
         <v>34</v>
@@ -3876,7 +3886,7 @@
         <v>114</v>
       </c>
       <c r="J36" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>114</v>
@@ -4729,6 +4739,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -4743,12 +4759,6 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A37">

</xml_diff>